<commit_message>
analysis for g-buffer optimization
</commit_message>
<xml_diff>
--- a/img/charts.xlsx
+++ b/img/charts.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="31">
   <si>
     <t>Number of Lights</t>
   </si>
@@ -39,6 +39,84 @@
   </si>
   <si>
     <t>Gbuffer Size - 2</t>
+  </si>
+  <si>
+    <t>gbuffer0</t>
+  </si>
+  <si>
+    <t>gbuffer1</t>
+  </si>
+  <si>
+    <t>gbuffer2</t>
+  </si>
+  <si>
+    <t>gbuffer3</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>pos.x</t>
+  </si>
+  <si>
+    <t>pox.y</t>
+  </si>
+  <si>
+    <t>pox.z</t>
+  </si>
+  <si>
+    <t>nothing</t>
+  </si>
+  <si>
+    <t>geomnor.x</t>
+  </si>
+  <si>
+    <t>geomnor.y</t>
+  </si>
+  <si>
+    <t>geomnor.z</t>
+  </si>
+  <si>
+    <t>color.g</t>
+  </si>
+  <si>
+    <t>color.b</t>
+  </si>
+  <si>
+    <t>color.r</t>
+  </si>
+  <si>
+    <t>normap.x</t>
+  </si>
+  <si>
+    <t>normap.y</t>
+  </si>
+  <si>
+    <t>normap.z</t>
+  </si>
+  <si>
+    <t>2_comp_normal.x</t>
+  </si>
+  <si>
+    <t>2_comp_normal.y</t>
+  </si>
+  <si>
+    <t>color.r &amp; normal sign</t>
+  </si>
+  <si>
+    <t>color.g &amp; normal axis</t>
+  </si>
+  <si>
+    <t>color.b &amp; normal axis</t>
   </si>
 </sst>
 </file>
@@ -91,6 +169,981 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Gbuffer size &amp; runtime</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> (ms)</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t> per</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> frame</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="7.4914260717410336E-2"/>
+          <c:y val="0.18097222222222226"/>
+          <c:w val="0.90286351706036749"/>
+          <c:h val="0.61498432487605714"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Gbuffer Size - 4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>22.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>83.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5A3A-4EEB-B629-8E63D3A08C7A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Gbuffer Size - 2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$C$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>20.399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-5A3A-4EEB-B629-8E63D3A08C7A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1178952319"/>
+        <c:axId val="1180522479"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1178952319"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1180522479"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1180522479"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1178952319"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>731520</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>51435</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>51435</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F3565E7B-8D4F-49AF-878D-8A95B5790874}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -390,19 +1443,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="16.734375" customWidth="1"/>
-    <col min="2" max="2" width="14.15625" customWidth="1"/>
+    <col min="2" max="2" width="20.734375" customWidth="1"/>
+    <col min="3" max="3" width="15.26171875" customWidth="1"/>
+    <col min="5" max="5" width="18.89453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -413,7 +1468,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
         <v>50</v>
       </c>
@@ -424,7 +1479,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <v>100</v>
       </c>
@@ -435,7 +1490,7 @@
         <v>30.3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <v>200</v>
       </c>
@@ -446,17 +1501,151 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17">
+        <v>0</v>
+      </c>
+      <c r="B17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" t="s">
+        <v>30</v>
+      </c>
+      <c r="E19" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>